<commit_message>
Add confirmation status to inquiry table and update related functionality
</commit_message>
<xml_diff>
--- a/uploads/inquiries/Inquiry_4.xlsx
+++ b/uploads/inquiries/Inquiry_4.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Ms1mQQBBT+qAsdblTxwpTS2fx6d9ell4dMIswkrQLfg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="B8Zjn2HREWuaK9hlGZGcCazgKuQoFPbMYUl47NR9QYo="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Product Name</t>
   </si>
@@ -27,25 +27,31 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>biscuits</t>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>MUTTON 1KG</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>Sugar 5kg</t>
+    <t>We can supply this all items tommorrow morning</t>
   </si>
   <si>
-    <t>test</t>
+    <t>BAIRAHA CHICKEN SUSAGES (500g)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>HALAL CHICKEN</t>
+  </si>
+  <si>
+    <t>BEEF 1KG</t>
   </si>
 </sst>
 </file>
@@ -310,13 +316,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.14"/>
+    <col customWidth="1" min="1" max="1" width="32.43"/>
     <col customWidth="1" min="2" max="2" width="9.14"/>
-    <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="9.14"/>
-    <col customWidth="1" min="5" max="5" width="13.71"/>
-    <col customWidth="1" min="6" max="6" width="13.0"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="14.14"/>
+    <col customWidth="1" min="4" max="4" width="20.43"/>
+    <col customWidth="1" min="5" max="5" width="45.86"/>
+    <col customWidth="1" min="6" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -335,27 +340,21 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2300.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -367,36 +366,47 @@
         <v>10.0</v>
       </c>
       <c r="C3" s="3">
-        <v>200.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>2000.0</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>750.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>850.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>150.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1500.0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2000.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>